<commit_message>
penambahan modul tambah jadwal
- restrukturisasi databse
- penambahan banyak view data (untuk mempermudah seleksi data)
- modul jadwal:
jadwal-view
jadwal-tambah
jadwal-delete
(untuk jadwal-view, tombol hapus masih di partial jadwal xi rpl, yang lain belum)
- modul pembagian mengajar
- modul tambah mapel

test-app sudah dihosting di https://moka.mdtsubululhuda.sch.id
</commit_message>
<xml_diff>
--- a/database/data_mapel.xlsx
+++ b/database/data_mapel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\moka-rc\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C00DD1E-9199-44DC-8302-97B4403730B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A6F0AA-0811-4FDD-B5E6-1EF40FB9B5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7433BF45-48B8-4926-B73B-A1607A3D6610}"/>
   </bookViews>
@@ -182,9 +182,6 @@
     <t>mapel</t>
   </si>
   <si>
-    <t>id_mapel</t>
-  </si>
-  <si>
     <t>XI</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Bahasa Inggris</t>
+  </si>
+  <si>
+    <t>nomor</t>
   </si>
 </sst>
 </file>
@@ -214,12 +214,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -234,8 +240,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FF1B12-3EA3-4387-9CF3-17DABAD1488C}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,61 +569,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>